<commit_message>
#83 std::format, datetime, timespan
 - x86 제거
 - cpp-terminal 적용
 - parallel_worker 100% 간헐적으로 안되는 현상 수정
 - 인코딩 삽질
</commit_message>
<xml_diff>
--- a/resources/table/const.xlsx
+++ b/resources/table/const.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\CSHYEON\Data\git\game\c++\fb\resources\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DB6D8B-DEDF-4F49-916D-A1127D9FE167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0CF828-43FA-4E69-B7DB-625EF8024176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2AD1A0EA-2C47-4BED-8190-24EDA4F164BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2AD1A0EA-2C47-4BED-8190-24EDA4F164BF}"/>
   </bookViews>
   <sheets>
     <sheet name="regex" sheetId="1" r:id="rId1"/>
@@ -161,108 +161,6 @@
     <t>이미 존재하는 이름입니다.</t>
   </si>
   <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 맵 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 정규표현식 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 월드맵 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 도어 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 스펠 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 워프 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 아이템 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 조합 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 판매 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 구매 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] NPC 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 몹 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 드롭 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] NPC 스폰 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 몹 스폰 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 클래스 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [%0.2lf%%] 게시판 정보를 읽었습니다. (%s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 맵 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 정규표현식 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 월드맵 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 도어 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 스펠 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 워프 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 아이템 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 조합 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 판매 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 구매 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 NPC 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 몹 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 드롭 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 NPC 스폰 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 몹 스폰 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 클래스 정보를 읽었습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * [100%%] 총 %d개의 게시판 정보를 읽었습니다.</t>
-  </si>
-  <si>
     <t>성별을 확인할 수 없습니다.</t>
   </si>
   <si>
@@ -847,6 +745,108 @@
   <si>
     <t>SILVER_BUNDLE</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 맵 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 정규표현식 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 월드맵 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 도어 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 스펠 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 워프 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 아이템 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 조합 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 판매 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 구매 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 NPC 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 몹 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 드롭 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 NPC 스폰 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 몹 스폰 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 클래스 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [100%] 총 %d개의 게시판 정보를 읽었습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 맵 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 정규표현식 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 월드맵 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 도어 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 스펠 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 워프 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 아이템 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 조합 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 판매 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 구매 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] NPC 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 몹 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 드롭 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] NPC 스폰 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 몹 스폰 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 클래스 정보를 읽었습니다. ({})</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * [{:0.2f}%] 게시판 정보를 읽었습니다. ({})</t>
   </si>
 </sst>
 </file>
@@ -1468,7 +1468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B64BF8E-904C-4727-916B-44450F4B2927}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1480,86 +1480,86 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>262</v>
+        <v>228</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>265</v>
+        <v>231</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>266</v>
+        <v>232</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>267</v>
+        <v>233</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>268</v>
+        <v>234</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>260</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>263</v>
+        <v>229</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>261</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -1572,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFB54FE-6D3B-49A4-815A-82E992FE6C32}">
   <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1587,7 +1587,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>0</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>0</v>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>0</v>
@@ -1750,12 +1750,12 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>0</v>
@@ -1764,12 +1764,12 @@
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>0</v>
@@ -1778,12 +1778,12 @@
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>45</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>0</v>
@@ -1792,12 +1792,12 @@
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>0</v>
@@ -1806,12 +1806,12 @@
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>0</v>
@@ -1820,12 +1820,12 @@
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>48</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>0</v>
@@ -1834,12 +1834,12 @@
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>49</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>0</v>
@@ -1848,12 +1848,12 @@
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>50</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>0</v>
@@ -1862,12 +1862,12 @@
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>51</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>0</v>
@@ -1876,12 +1876,12 @@
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>52</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>0</v>
@@ -1890,12 +1890,12 @@
         <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>53</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>0</v>
@@ -1904,12 +1904,12 @@
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>54</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>0</v>
@@ -1918,12 +1918,12 @@
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>55</v>
+        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>0</v>
@@ -1932,12 +1932,12 @@
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>56</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>0</v>
@@ -1946,12 +1946,12 @@
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>57</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>0</v>
@@ -1960,12 +1960,12 @@
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>58</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>0</v>
@@ -1974,12 +1974,12 @@
         <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>59</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>0</v>
@@ -1988,12 +1988,12 @@
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>60</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>0</v>
@@ -2002,12 +2002,12 @@
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>61</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>0</v>
@@ -2016,12 +2016,12 @@
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>62</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>0</v>
@@ -2030,12 +2030,12 @@
         <v>1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>63</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>0</v>
@@ -2044,12 +2044,12 @@
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>64</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>0</v>
@@ -2058,12 +2058,12 @@
         <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>65</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>0</v>
@@ -2072,12 +2072,12 @@
         <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>0</v>
@@ -2086,12 +2086,12 @@
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>67</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>0</v>
@@ -2100,12 +2100,12 @@
         <v>1</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>68</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>0</v>
@@ -2114,12 +2114,12 @@
         <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>69</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>0</v>
@@ -2128,12 +2128,12 @@
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>70</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>0</v>
@@ -2142,12 +2142,12 @@
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>71</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>0</v>
@@ -2156,12 +2156,12 @@
         <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>72</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>0</v>
@@ -2170,12 +2170,12 @@
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>0</v>
@@ -2184,12 +2184,12 @@
         <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>74</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>0</v>
@@ -2198,12 +2198,12 @@
         <v>1</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>75</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>0</v>
@@ -2212,12 +2212,12 @@
         <v>1</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>76</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>0</v>
@@ -2226,12 +2226,12 @@
         <v>1</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>0</v>
@@ -2240,12 +2240,12 @@
         <v>1</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>0</v>
@@ -2254,12 +2254,12 @@
         <v>1</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>0</v>
@@ -2268,12 +2268,12 @@
         <v>1</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>0</v>
@@ -2282,12 +2282,12 @@
         <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>0</v>
@@ -2296,12 +2296,12 @@
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>0</v>
@@ -2310,12 +2310,12 @@
         <v>1</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>0</v>
@@ -2324,12 +2324,12 @@
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>0</v>
@@ -2338,12 +2338,12 @@
         <v>1</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>0</v>
@@ -2352,12 +2352,12 @@
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>0</v>
@@ -2366,12 +2366,12 @@
         <v>1</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>0</v>
@@ -2380,12 +2380,12 @@
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>0</v>
@@ -2394,12 +2394,12 @@
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>0</v>
@@ -2408,12 +2408,12 @@
         <v>1</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>0</v>
@@ -2422,12 +2422,12 @@
         <v>1</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>0</v>
@@ -2436,12 +2436,12 @@
         <v>1</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>0</v>
@@ -2450,12 +2450,12 @@
         <v>1</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>0</v>
@@ -2464,12 +2464,12 @@
         <v>1</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>205</v>
+        <v>171</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>0</v>
@@ -2478,12 +2478,12 @@
         <v>1</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>0</v>
@@ -2492,12 +2492,12 @@
         <v>1</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>0</v>
@@ -2506,12 +2506,12 @@
         <v>1</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>0</v>
@@ -2520,12 +2520,12 @@
         <v>1</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>0</v>
@@ -2534,12 +2534,12 @@
         <v>1</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>210</v>
+        <v>176</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>0</v>
@@ -2548,12 +2548,12 @@
         <v>1</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>211</v>
+        <v>177</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>0</v>
@@ -2562,12 +2562,12 @@
         <v>1</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>0</v>
@@ -2576,12 +2576,12 @@
         <v>1</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>213</v>
+        <v>179</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>0</v>
@@ -2590,12 +2590,12 @@
         <v>1</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>0</v>
@@ -2604,12 +2604,12 @@
         <v>1</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>0</v>
@@ -2618,12 +2618,12 @@
         <v>1</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>216</v>
+        <v>182</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>0</v>
@@ -2632,12 +2632,12 @@
         <v>1</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>0</v>
@@ -2646,12 +2646,12 @@
         <v>1</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>0</v>
@@ -2660,12 +2660,12 @@
         <v>1</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>0</v>
@@ -2674,12 +2674,12 @@
         <v>1</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>220</v>
+        <v>186</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>0</v>
@@ -2688,12 +2688,12 @@
         <v>1</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>0</v>
@@ -2702,12 +2702,12 @@
         <v>1</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>222</v>
+        <v>188</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>0</v>
@@ -2716,12 +2716,12 @@
         <v>1</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>223</v>
+        <v>189</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>0</v>
@@ -2730,12 +2730,12 @@
         <v>1</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>0</v>
@@ -2744,12 +2744,12 @@
         <v>1</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>0</v>
@@ -2758,12 +2758,12 @@
         <v>1</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>226</v>
+        <v>192</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>0</v>
@@ -2772,12 +2772,12 @@
         <v>1</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>0</v>
@@ -2786,12 +2786,12 @@
         <v>1</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>228</v>
+        <v>194</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>0</v>
@@ -2800,12 +2800,12 @@
         <v>1</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>229</v>
+        <v>195</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>0</v>
@@ -2814,12 +2814,12 @@
         <v>1</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>230</v>
+        <v>196</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>0</v>
@@ -2828,12 +2828,12 @@
         <v>1</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>0</v>
@@ -2842,12 +2842,12 @@
         <v>1</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>0</v>
@@ -2856,12 +2856,12 @@
         <v>1</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>233</v>
+        <v>199</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>0</v>
@@ -2870,12 +2870,12 @@
         <v>1</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>234</v>
+        <v>200</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>0</v>
@@ -2884,12 +2884,12 @@
         <v>1</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>0</v>
@@ -2898,12 +2898,12 @@
         <v>1</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>236</v>
+        <v>202</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>0</v>
@@ -2912,12 +2912,12 @@
         <v>1</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>0</v>
@@ -2926,12 +2926,12 @@
         <v>1</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>0</v>
@@ -2940,12 +2940,12 @@
         <v>1</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>0</v>
@@ -2954,12 +2954,12 @@
         <v>1</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>0</v>
@@ -2968,12 +2968,12 @@
         <v>1</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>241</v>
+        <v>207</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>0</v>
@@ -2982,12 +2982,12 @@
         <v>1</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>0</v>
@@ -2996,12 +2996,12 @@
         <v>1</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>243</v>
+        <v>209</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>0</v>
@@ -3010,12 +3010,12 @@
         <v>1</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>0</v>
@@ -3024,12 +3024,12 @@
         <v>1</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>0</v>
@@ -3038,12 +3038,12 @@
         <v>1</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>0</v>
@@ -3052,12 +3052,12 @@
         <v>1</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>247</v>
+        <v>213</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>0</v>
@@ -3066,12 +3066,12 @@
         <v>1</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>0</v>
@@ -3080,12 +3080,12 @@
         <v>1</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>0</v>
@@ -3094,12 +3094,12 @@
         <v>1</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>0</v>
@@ -3108,12 +3108,12 @@
         <v>1</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>0</v>
@@ -3122,12 +3122,12 @@
         <v>1</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>0</v>
@@ -3136,7 +3136,7 @@
         <v>1</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3160,16 +3160,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>254</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>